<commit_message>
change the realisation of the cell iteration
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/test_example.xlsx
+++ b/src/main/resources/templates/excel/test_example.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="108">
   <si>
     <t>BASIC INFO</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>1Arab National Bank</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1083,7 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1205,6 +1208,9 @@
       <c r="A2" t="s">
         <v>53</v>
       </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
       <c r="D2" t="s">
         <v>106</v>
       </c>
@@ -1280,7 +1286,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
roughly processing of the second page
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/test_example.xlsx
+++ b/src/main/resources/templates/excel/test_example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="27700" windowHeight="17560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="27700" windowHeight="17560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DESCRIPTION" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="190">
   <si>
     <t>BASIC INFO</t>
   </si>
@@ -235,9 +235,6 @@
     <t>COMPANY</t>
   </si>
   <si>
-    <t>NO LIMIT TO NUMBER OF ITEMS</t>
-  </si>
-  <si>
     <t>ROBERT</t>
   </si>
   <si>
@@ -401,6 +398,556 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Arabia Insurance Cooperative Co</t>
+  </si>
+  <si>
+    <t>Najm for Insurance Services</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>10 January 2016</t>
+  </si>
+  <si>
+    <t>Arabia Insurance gets SAMA's nod for 11 products</t>
+  </si>
+  <si>
+    <t>https://english.mubasher.info/news/2888887/Arabia-Insurance-gets-SAMA-s-nod-for-11-products</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3 August 2014</t>
+    </r>
+  </si>
+  <si>
+    <t>Arabia Insurance says Mais Medical Products warehouse caught fire</t>
+  </si>
+  <si>
+    <t>https://english.mubasher.info/news/2576821/Arabia-Insurance-says-Mais-Medical-Products-warehouse-caught-fire</t>
+  </si>
+  <si>
+    <t>3 February 2013</t>
+  </si>
+  <si>
+    <t>AICC obtains final approval to sell two insurance products (TASI)</t>
+  </si>
+  <si>
+    <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=52966</t>
+  </si>
+  <si>
+    <t>AICC renews license of 17 products (TASI)</t>
+  </si>
+  <si>
+    <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=52056</t>
+  </si>
+  <si>
+    <t>AICC extends a license for two products (TASI)</t>
+  </si>
+  <si>
+    <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=50755</t>
+  </si>
+  <si>
+    <t>AICC obtains an approval to sell two insurance products (TASI)</t>
+  </si>
+  <si>
+    <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=49854</t>
+  </si>
+  <si>
+    <t>7 January 2012</t>
+  </si>
+  <si>
+    <t>AICC extends the temporary approval to sell and market 22 products (TASI)</t>
+  </si>
+  <si>
+    <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=44228</t>
+  </si>
+  <si>
+    <t>AICC in the process of opening 25 selling points in Saudi Arabia (TASI)</t>
+  </si>
+  <si>
+    <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=44229</t>
+  </si>
+  <si>
+    <t>National Health Insurance Network opened for AICC (TASI)</t>
+  </si>
+  <si>
+    <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=39100</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>16 August 2010</t>
+    </r>
+  </si>
+  <si>
+    <t>AICC concludes vehicles insurance agreement with National Bank (TASI)</t>
+  </si>
+  <si>
+    <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=33634</t>
+  </si>
+  <si>
+    <t>13 March 2010</t>
+  </si>
+  <si>
+    <t>Arab Insurance Co to extended temporary approval to sell and market 25 insurance products (TASI)</t>
+  </si>
+  <si>
+    <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=18135</t>
+  </si>
+  <si>
+    <t>https://www.tadawul.com.sa/wps/portal/tadawul/market-participants/issuers/issuers-directory/company-details/!ut/p/z1/pdFLb4JAFAXg3-KC9RyGZ90hICBIQhWlszGDTRDDK4ba-O87Wjckldb07m7yncW5lzCSEdbwc1nwvmwbXon9jem72I9sHyYNPXetwNKdpf0aBxQA2d4ApbYpv6iIEBmyAB6CZKkqSBTCnsp7QWzASix_M98IatL_5aH-LY8HY-H3PBsS-NQRxA1Dx9YoZtodjJ1oCH64wSi4lryBkRYLwoqqzb8_euj7bipBQs_f-edHJYmW-7bueHNZXeq8FciUdZAVP5GuTtM0QxkctepcTCZf8Uoyeg!!/dz/d5/L0lHSkovd0RNQU5rQUVnQSEhLzROVkUvZW4!/</t>
+  </si>
+  <si>
+    <t>https://ar.wikipedia.org/wiki/%D8%B4%D8%B1%D9%83%D8%A9_%D8%A7%D9%84%D8%AA%D8%A3%D9%85%D9%8A%D9%86_%D8%A7%D9%84%D8%B9%D8%B1%D8%A8%D9%8A%D8%A9_%D8%A7%D9%84%D8%AA%D8%B9%D8%A7%D9%88%D9%86%D9%8A%D8%A9</t>
+  </si>
+  <si>
+    <t>http://www.aicc.com.sa/</t>
+  </si>
+  <si>
+    <t>https://www.mubasher.info/markets/TDWL/stocks/8240/profile</t>
+  </si>
+  <si>
+    <t>http://www.aicc.com.sa/section.aspx?idc=19&amp;id=2</t>
+  </si>
+  <si>
+    <t>Arabian Pipes Co.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>22 July 2018</t>
+  </si>
+  <si>
+    <t>The Arab Pipe Company announces its winning a contract for the supply of pipes to Saudi Aramco worth more than 139 million riyals</t>
+  </si>
+  <si>
+    <r>
+      <t>https://www.argaam.com/en/article/articledetail/id/561475</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/jZBNj4IwEIZ_yx44z9AFdfeGDYoidVc-hF5IUaMktHCoa_z3dvEMOrdJnvedJwMccuBK_NVnoetWicbsBZ-ULNjQAGckxIQt0PvNtnQe-WEaTmDfA4TQmf3l4Ga5YlMDeEG2yJJPRAf4O3kcGA9f53mPjBn0wNiJ8QYXCiM5HbQgBOL_Do-xbcqoH_ksKVkazf0dFK7tIsIa-Llpq-dDL1p33xZaqMVR3K6NZQyEUlRoyO0h4NDKTqh7fJdVa1oIMa3xSUEn0xzrHynLSLuV8_EAdM-FkA!!/dz/d5/L0lHSkovd0RNQURrQUVnQSEhLzROVkUvYXI!/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://english.mubasher.info/news/3317076/Saudi-Steel-Pipe-Arabian-Pipes-to-provide-Aramco-with-steel-pipes</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=73659</t>
+    </r>
+  </si>
+  <si>
+    <t>Arabian Pipes Company awarded SR 261 million order for the supply of steel pipes to Saudi Aramco</t>
+  </si>
+  <si>
+    <r>
+      <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pZJPc6JAEMU_Sw4eU9MzMEj2hsMICIwLMipcLGJIYpX8KYOm9NPvBK1apTbxsNzo-b3uV68bZWiJsio_bN7ydlNX-Vb9p5mxEm7AXDCJD4kYgxXNp2wUcl_6Blp0ACHMxE86BBAMMViGA14U6hpEGsqu9Q5PNPVshywWHgGAvt7xxFANsNz5eK5Qk_yfHvRb_V3_Pb2j9fUcwAqnk3FMJ9gMAKVKP7wCpHxSBjUWRTYl4FA0QxnKPop8t36P9sXuiFJCOt9Zr7VLbKXkvm8zpRzRC_BTtLfAP7L7EfgKpwPgm8-CC-D9dnTsKZNmYozAkiwQtphhoMadEc49k0DRBGVv2_r5fGzvbdv8GsAA2vwl_9xvB8rCui6bvDrOjuVzraAuvm_QvKpY3qIlvuzlr3Hhq8Ph2AfdDTHoOpJVvSvV0MVhU3xebyk5NgVK8VdBtav367Ko2ktx9djVP85WzpvsX8DtiRFy7m0JMZWC8ZCLZCVkOOIxSinodIiaUkq5PCWvDY957J6CYvGYTg6CHk6JZT08_AHrKaY8/dz/d5/L0lDUmlTUSEhL3dHa0FKRnNBLzROV3FpQSEhL2Vu/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.argaam.com/en/article/articledetail/id/545327</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://kallanish.com/en/steel-news/market-reports/article-details/arabian-pipes-wins-large-aramco-contract-0418/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://english.mubasher.info/news/3271623/Arabian-Pipes-wins-SAR-261m-contract-from-Aramco</t>
+    </r>
+  </si>
+  <si>
+    <t>Arabian Pipes Company has been awarded an order value exceeding SR 173 million to supply OCTG pipes for Saudi Aramco.</t>
+  </si>
+  <si>
+    <r>
+      <t>https://www.marketscreener.com/ARABIAN-PIPES-COMPANY-6498187/news/Arabian-Pipes-Company-has-been-awarded-an-order-value-exceeding-SR-173-million-to-supply-OCTG-pipe-25595909/?iCStream=1</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/hZBLb4MwEIR_Sw8cq10M4dEbcUlwAOdhoOBLZNqKRuKlijbKv6-TXnoh3dtoZr8dLUgoQfbq-9So6TT0qtW6ks6RRwmN0CMxZnyFwb7Y0mUaxnnswAtU2kdaHJhNcL0rFsjsRBCx21jICMg_rheJZ2Tx3nKtVMvEvG7rACHUM30bkzXjrsYHUbEqMgvRBnn_ulCfwKOhe9ckeQvfY90CODMB_kdYQKXrurN9CAFxZQScb3NOwzTk2ZHn6TI8QGV7ju_DBmTTDvXvYz-maXwy0MBJvanzV2voBqrvqZqgNOcCr0M3qv4iLl09aAohiDB2eXkW7FHV3sVqm4cfe1-oLQ!!/dz/d5/L0lHSkovd0RNQUprQUVnQSEhLzROVkUvZW4!/</t>
+    </r>
+  </si>
+  <si>
+    <t>Arabian Pipes Company awarded SR 78 million orders for the supply of steel pipes to Saudi Aramco</t>
+  </si>
+  <si>
+    <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/hZFLU4NAEIR_DecdNrBBb8vKGxYNj8BeUhu1IhavA8aKv94N8aIWydym6uue7hokUIVEL4_NQU7N0MtW7bUgO-7HzAcLR5BzF-hTmTI7caIiImg7AxgzS78zIPYCvlYA9Uu3zFfgrZD4rXcAaJKG7sYMdSuGG3ow_ur_3xczEjx6hh4oxMqJDbRgMX_gmQ4m-QGuRbwKnDPMACwMhVsOJqpVzfViD4xRdvagnKcFZ07i8HzHi8R2Nqg2CCEWCpE4tMP-8pK3aRrvNdBgki_y86PVVALZ90xOqNKXgOehG2V_yk7dflAuGAOgsSsqaIJ3czx-xa9b-g3cxkle/dz/d5/L0lDUmlTUSEhL3dHa0FKRnNBLzROV3FpQSEhL2Vu/</t>
+  </si>
+  <si>
+    <t>12 March 2017</t>
+  </si>
+  <si>
+    <t>Arabian Pipes Company awarded SR 135 million order for the supply of OCTG steel pipes to Saudi Aramco</t>
+  </si>
+  <si>
+    <r>
+      <t>https://www.argaam.com/en/article/articledetail/id/474286</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pdFdT4MwFIDhX8P1OSswmHe1IEUYSceYozemm-wj4SuTadivt6KJWaIzy3rX5HnbnBYkLEHW6m2_Vd2-qVWp97kcPyc8ZhxdEgX-3EQ69qZsloQEEeFpAIQwdzSxMMbYGWkQYCimlonCBHlVH4SJg1RQvnhYaOqS23q0_utz3Ts_ALNsooHJhPBsgoENKUiQr4U6rHfiWBx6yAkZ7pXnRyMnni79KPKYLu_tb3Dpac7BL7NfBJ_DDQD_WBThEeS2bFZfP7nruvbOQAM79aLej6WBINdN1aq6T_tq1Wg0zJYWNbRVli1P803rz_gp3tAPpgjskQ!!/dz/d5/L0lDU0lKQ2dwUkNpQ2xFQSEvb01vUUFBSVF4QkFJRW95akNVNXdYQlNnakhBIS80SkNpanNZcE1oVGpVRTF1MGxzcHFhUSEvWjdfTkhMQ0gwODJLMFRORjBBUVZPQ0JNRUtVMjIvWjZfTkhMQ0gwODJLMFRORjBBUVZPQ0JNRUtVSzYvQU5OT1VOQ0VNRU5UX05VTUJFUi80NTkxNS9odHRwOiUwJTB0YWRhd3VsJTAvYW5uQ2F0LzE!/</t>
+    </r>
+  </si>
+  <si>
+    <t>Arabian Pipes Company awarded SR 72 million order for the supply of OCTG steel pipes to Saudi Aramco</t>
+  </si>
+  <si>
+    <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/hZBRT4MwFIV_yx543b0rbEPfOsJENzp1wKAvS1FkJKMQ7CT46y2YmJiIa596-52Tew5wiIFL8VHkQhWVFGf9TvjiyLyt46FNNhiwNdKnaOesfHcTbhZwGABCHHt2Y-H27p4tNUC9aB0FJqIF_JqeD8h_DgOAI4fiNYc5PADPz1X6nYfK1LRz4E32ljVZM700enxSqr410MC2bacE-zuVmTLwL8WpelcQ_yZ77sdEiVfRXs5azYWUjtC_szHgpSprIbt9V6aVXoQQREh0qcvR1giBfZ-ZMrYLmeP6LguOLPRX7jMklqVLgLqMsXgsD7aap535GVA6mXwBPc2OSw!!/dz/d5/L0lDUmlTUSEhL3dHa0FKRnNBLzROV3FpQSEhL2Vu/</t>
+  </si>
+  <si>
+    <t>Arabian pipes company been awarded SR 78 million orders for the supply of steel pipes to Saudi Aramco</t>
+  </si>
+  <si>
+    <r>
+      <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pZFNc4IwEIZ_iwfOWcJne4MQgQKxKCDk4sR2xjLD1yGt479vtB6qo_bQvWX2eXfffYM4qhEfxFe7E7IdB9Gpd8PtDYtSEoGLEyjYHLy8WhA_o0mZ2Gh9AjAmrv5kQgqpo4NnhxDnmWlAbiD-Wx_SwlDtICNLFmMAuNaHMXPUAi-q5pVCXfw_PZiX-lv--RUS4UCtoEkSEAuDb52BRydeAjdueAgcTZ4AuFMe_DXBQi-I77px-_NlH1JOzxpoIMW72H92mhrwNvaTGA6rQ78dFYRVevdQMQxESFTrqFHpOnfjwxitjs48xhYlIzSjrNiwMvPpEjWmaRkOmvqyrKGN29d-7UoX9t5s9g1W0E1t/dz/d5/L0lDUmlTUSEhL3dHa0FKRnNBLzROV3FpQSEhL2Vu/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=71125</t>
+    </r>
+  </si>
+  <si>
+    <t>27 June 2016</t>
+  </si>
+  <si>
+    <t>Arabian Pipes wins pipe pact from Saudi Aramco</t>
+  </si>
+  <si>
+    <t>http://www.kallanishenergy.com/2016/06/27/arabian-pipes-wins-pipe-pact-saudi-aramco/</t>
+  </si>
+  <si>
+    <t>Arabian Pipes Co. wins OCTG and welded steel pipes orders from Aramco</t>
+  </si>
+  <si>
+    <t>https://www.scmdaleel.com/article/arabian-pipes-co-wins-octg-and-welded-steel-pipes-orders-from-aramco/370</t>
+  </si>
+  <si>
+    <t>Arabian pipes company awarded SR 21 million project for the supply of steel pipes to Saudi Aramco</t>
+  </si>
+  <si>
+    <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pVFNb4IwGP4tO3hc-rZUxN0qQ0GgbgIqXExxRFmgEEUN-_WraLJkifOw3vrk-WxRglYokeKUb0WTV1IU6h4n-prbnmmDQVwI-RjY-2JmjnzLjVwdLTsCIaaBhxS8icMHisDsxXgRagAUJf_RT7TfeguA-bPpeN6fYsMDpU86yl8NOgLcOQweOfRvBOdtQrGjWhihPgIWmR5_5QGGvv7AQa0IxB7Faurg7lsQgoKLD-N8FnHT8i0ernnkj6w5iikeEoqmKNkWVXr9ll3T1C896EEjPsT5WPTUDiGlKRq0wvcIm6qshWyDtkwr5UIIwK3WzzjuasAs7AK1fQyUokhW-1KFLk95dr6WPGRiv9mFbZ2hGF8AlVwdN2Ummxu4fu7wwzUp7pLqMlpB7nxSkRqtVpxKM_3KYvb0Df21EUM!/dz/d5/L0lHSkovd0RNQUZrQUVnQSEhLzROVkUvZW4!/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arabian Pipes Company awarded SR 9 Million project for the supply of OCTG Steel Pipes to Saudi Aramco </t>
+  </si>
+  <si>
+    <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pVFNb4IwGP4tO3hc-rZUZLtVhoJA3QRUuJjiiLJAIYoa_PWraLJkifOw3vrk-WxRgpYokeKYb0STV1IU6h4n-orbnmmDQVwI-QjYx3xqDn3LjVwdLToCIaaBXyh4Y4cPFIHZ89E81AAoSv6jH2u_9RYA86eT0aw_wYYHSp90lL8adAS4cxg8cujfCM77mGJHtTBCfQgsMj3-xgMMff2Bg1oRiB2K1dTB3bcgBAUXH8b5NOKm5Vs8XPHIH1ozFFNsUA1NULIpqvT6LdumqV970INGfIrToeipHUJKUzRoie8R1lVZC9kGbZlWyoUQgFutn3Hc1YBZ2AVq-xgoRZGsdqUKXRzz7HQtuc_Ebr0N2zpDMb4AKrk6rMtMNjdw9dzh-2tS3CXVZbSE3PmiIjVarTiWZnrOYvb0DZ3SUsU!/dz/d5/L0lHSkovd0RNQUZrQUVnQSEhLzROVkUvZW4!/</t>
+  </si>
+  <si>
+    <t>30 March 2016</t>
+  </si>
+  <si>
+    <t>Arabian pipes company awarded SR 73 million project for the supply of steel pipes to Saudi Aramco</t>
+  </si>
+  <si>
+    <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pVFNb4IwGP4tO3hc-rZUZLtVhoJA3QRUuJjiiLJAIYoa_PWraLJkifOw3vrk-WxRgpYokeKYb0STV1IU6h4n-orbnmmDQVwI-QjYx3xqDn3LjVwdLToCIaaBXyh4Y4cPFIHZ89E81AAoSv6jH2u_9RYA86eT0aw_wYYHSp90lL8adAS4cxg8cujfCM77mGJHtTBCfQgsMj3-xgMMff2Bg1oRiB2K1dTB3bcgBAUXH8b5NOKm5Vs8XPHIH1ozFFNsgIYmKNkUVXr9lm3T1K896EEjPsXpUPTUDiGlKRq0xPcI66qshWyDtkwr5UIIwK3WzzjuasAs7AK1fQyUokhWu1KFLo55drqW3Gdit96GbZ2hGF8AlVwd1mUmmxu4eu7w_TUp7pLqMlpC7nxRkRqtVhxLMz1nMXv6Bp_kZcA!/dz/d5/L0lHSkovd0RNQUZrQUVnQSEhLzROVkUvZW4!/</t>
+  </si>
+  <si>
+    <t>28 February 2016</t>
+  </si>
+  <si>
+    <t>Arabian pipes company awarded SR 42 million project for the supply of steel pipes to Al Robaya Holding co.</t>
+  </si>
+  <si>
+    <r>
+      <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pVFNb4IwGP4tO3hc-rYUZLvVDgWBugmocDHFEWXhK4ou7NevosmSJc7DeuuT57NFCVqhpJKnfCvbvK5koe5xYqyF7XEbTOJCKMbA3hYzPvItN3INtOwJhHATP1HwJo4YKgKzF-NFqAFQlPxHP9F-6y0A5s-m47k-xaYHSp_0lL8a9AS4cRjcc9CvBOd1QrGjWpihMQIWcU-8iACDbtxxUCsCuUexmjq8-RaEoODsw4SYRYJbviXCtYj8kTVHMcWU6miKkm1Rp5dv2bVt8zyAAbTyXX4ei4HaIauKyxat8C3Cpi4bWXVBV6a1ciEE4FrrZ5xwNWAWdoHaPgZKUVTV-1KFLk959nkpecjkfrMLuyZDMT4DKrk-bsqsaq_g-rHHD5ekuE9qymgFufNBZWp2WnEqefqVxezhG_Y0V-0!/dz/d5/L0lHSkovd0RNQUZrQUVnQSEhLzROVkUvZW4!/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=68410</t>
+    </r>
+  </si>
+  <si>
+    <t>Arabian pipes company awarded SR 68 million project for the supply of steel pipes to Saudi Aramco</t>
+  </si>
+  <si>
+    <r>
+      <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pVFNb4IwGP4tO3hc-rZUZLtVhoJA3QRUuJjiiLJAIYoa_PWraLJkifOw3vrk-WxRgpYokeKYb0STV1IU6h4n-orbnmmDQVwI-QjYx3xqDn3LjVwdLToCIaaBXyh4Y4cPFIHZ89E81AAoSv6jH2u_9RYA86eT0aw_wYYHSp90lL8adAS4cxg8cujfCM77mGJHtTBCfQgsMj3-xgMMff2Bg1oRiB2K1dTB3bcgBAUXH8b5NOKm5Vs8XPHIH1ozFFMgmKAJSjZFlV6_Zds09WsPetCIT3E6FD21Q0hpigYt8T3CuiprIdugLdNKuRACcKv1M467GjALu0BtHwOlKJLVrlShi2Oena4l95nYrbdhW2coxhdAJVeHdZnJ5gaunjt8f02Ku6S6jJaQO19UpEarFcfSTM9ZzJ6-AQ0RLfU!/dz/d5/L0lHSkovd0RNQUZrQUVnQSEhLzROVkUvZW4!/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=66830</t>
+    </r>
+  </si>
+  <si>
+    <t>13 October 2015</t>
+  </si>
+  <si>
+    <t>Arabian pipes company awarded SR 38 million project for the supply of steel pipes to Saudi Aramco</t>
+  </si>
+  <si>
+    <r>
+      <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pVFNb4IwGP4tO3hc-hYq4m61Q0GgbgIqXExxRFmgEEUN-_WraLJkifOw3vrk-WxRglYokeKUb0WTV1IU6h4nxprbHrPB1FwI-Rjo-2LGRr7lRq6Blh1B05iJhwS8icMHikDtxXgR6gAEJf_RT_TfeguA-rPpeN6fYtMDpU86yl8NOgLcORQeOfRvBOdtQrCjWpihMQIaMY-_8gBD33jgoFYEYo9iNXVw9y00DQUXH8r5LOLM8i0ernnkj6w5ivWhaWA0Rcm2qNLrt-yapn7pQQ8a8SHOx6KndggpmWjQCt8jbKqyFrIN2jKtlIumAdxq_Yzjrg7Uwi4Q28dACIpktS9V6PKUZ-dryUMm9ptd2NYZivEFUMnVcVNmsrmB6-cOP1yT4i6pLqMV5M4nEanZ6sWpZOlXFtOnb-sKc60!/dz/d5/L0lHSkovd0RNQUZrQUVnQSEhLzROVkUvZW4!/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=65959</t>
+    </r>
+  </si>
+  <si>
+    <t>7 October 2015</t>
+  </si>
+  <si>
+    <r>
+      <t>https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pVFNb4IwGP4tO3hc-rZ8iLvVDgWBugmocDHFEWXhK4oa9utXwWTJEudhvfXJ89miGK1RXIpzthNNVpUil_co1jfccpkFBnEg4BOg78s5G3umEzo6WnUEQpiBRyq4U5sPJYFay8kyUABUFP9HP1V-600A6s1nk4U2w4YLUh93lL8adAS4cyg8ctBuBPttqmJbtjACfQw0ZC5_5T4GTX_gIFf44oAiOXV49y0IQf7Vh3I-DzkzPZMHGx56Y3OBImU0HGlohuJdXiX9t-ybpn4ZwAAa8SEup3wgd4iyZKJBa3yPsK2KWpSt3xZJJV0IAbjV-hnHHQWoiR1QLQ-DqqKwrA6FDF2ds_TSlzym4rDdB22doghfAZlcnbZFWjY3cPPc4cc-KeqS6iJcQ2Z_qiIxWiU_Fyz5SiP69A1PlXYz/dz/d5/L0lHSkovd0RNQUZrQUVnQSEhLzROVkUvZW4!/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://www.asmainfo.com/Saudi/En/news/shownews.aspx?rid=65812</t>
+    </r>
+  </si>
+  <si>
+    <t>23 March 2015</t>
+  </si>
+  <si>
+    <t>Imposition of a Penalty on the Arabian Pipes Company</t>
+  </si>
+  <si>
+    <t>https://cma.org.sa/en/Market/NEWS/Pages/CMA_N_1716.aspx</t>
+  </si>
+  <si>
+    <t>Arabian Pipes acquires Arabian-Yadong</t>
+  </si>
+  <si>
+    <t>https://english.mubasher.info/news/2623151/Arabian-Pipes-acquires-Arabian-Yadong</t>
+  </si>
+  <si>
+    <t>Arabian Pipes wins SAR 58 mln contract from Aramco</t>
+  </si>
+  <si>
+    <t>https://english.mubasher.info/news/2603212/Arabian-Pipes-wins-SAR-58-mln-contract-from-Aramco</t>
   </si>
 </sst>
 </file>
@@ -410,17 +957,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -477,6 +1017,46 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -507,27 +1087,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -536,8 +1116,25 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1082,7 +1679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1090,7 +1687,7 @@
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
@@ -1109,7 +1706,7 @@
     <col min="19" max="19" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="16.5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="80.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5" style="8" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7.5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.5" bestFit="1" customWidth="1"/>
@@ -1127,7 +1724,7 @@
       <c r="B1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -1143,10 +1740,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>6</v>
@@ -1155,10 +1752,10 @@
         <v>7</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>8</v>
@@ -1167,7 +1764,7 @@
         <v>33</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>9</v>
@@ -1187,7 +1784,7 @@
       <c r="V1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="9" t="s">
         <v>34</v>
       </c>
       <c r="X1" s="6" t="s">
@@ -1206,156 +1803,156 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
       <c r="D2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" s="16">
+        <v>105</v>
+      </c>
+      <c r="E2" s="15">
         <v>10000000000</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="15">
         <v>1000000000</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" t="s">
+        <v>94</v>
+      </c>
+      <c r="O2" t="s">
         <v>60</v>
       </c>
-      <c r="K2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" t="s">
-        <v>98</v>
-      </c>
-      <c r="M2" t="s">
-        <v>99</v>
-      </c>
-      <c r="N2" t="s">
-        <v>95</v>
-      </c>
-      <c r="O2" t="s">
-        <v>61</v>
-      </c>
-      <c r="P2" s="11">
+      <c r="P2" s="10">
         <v>4170</v>
       </c>
-      <c r="Q2" s="12">
+      <c r="Q2" s="11">
         <v>29190</v>
       </c>
       <c r="R2" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" t="s">
         <v>63</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>64</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>65</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>66</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>67</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>68</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>69</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>70</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="16">
+        <v>99</v>
+      </c>
+      <c r="E3" s="15">
         <v>1111111111111</v>
       </c>
       <c r="F3">
         <v>11</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <v>101231230</v>
       </c>
       <c r="H3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" s="16">
+        <v>31974</v>
+      </c>
+      <c r="K3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N3" t="s">
         <v>101</v>
       </c>
-      <c r="I3" t="s">
-        <v>105</v>
-      </c>
-      <c r="J3" s="17">
-        <v>31974</v>
-      </c>
-      <c r="K3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" t="s">
-        <v>98</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="10">
+        <v>100</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>29190</v>
+      </c>
+      <c r="R3" t="s">
         <v>103</v>
       </c>
-      <c r="N3" t="s">
-        <v>102</v>
-      </c>
-      <c r="O3" t="s">
-        <v>61</v>
-      </c>
-      <c r="P3" s="11">
-        <v>100</v>
-      </c>
-      <c r="Q3" s="12">
-        <v>29190</v>
-      </c>
-      <c r="R3" t="s">
-        <v>104</v>
-      </c>
       <c r="S3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" t="s">
         <v>64</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>65</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>66</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
         <v>67</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>68</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>69</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>70</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1372,10 +1969,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1411,338 +2008,1015 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="13">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="14">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="13">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="14">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="14">
+      <c r="C4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="13">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.871</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="14">
-        <v>0.871</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
         <v>53</v>
       </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="14">
+        <v>78</v>
+      </c>
+      <c r="D6" s="13">
         <v>0.4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>52</v>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" t="s">
-        <v>54</v>
+      <c r="C8" s="14">
+        <v>43354</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>48</v>
+      <c r="C9" s="14">
+        <v>43326</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="15">
-        <v>43354</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>81</v>
+      <c r="C10" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="15">
-        <v>43326</v>
+      <c r="C11" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>84</v>
+      <c r="C12" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>87</v>
+      <c r="C13" s="14">
+        <v>43202</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>81</v>
+      <c r="C14" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="15">
-        <v>43202</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
         <v>53</v>
       </c>
-      <c r="B16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
         <v>53</v>
       </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="17">
+        <v>3.85E-2</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="14">
+        <v>41251</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="14">
+        <v>41182</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="14">
+        <v>41123</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="14">
+        <v>40660</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>52</v>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="14">
+        <v>43219</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" s="14">
+        <v>43069</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" s="14">
+        <v>42852</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="14">
+        <v>42724</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="14">
+        <v>42683</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="14">
+        <v>42473</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" s="14">
+        <v>42466</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>143</v>
+      </c>
+      <c r="C54" s="14">
+        <v>42463</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" s="14">
+        <v>42319</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" t="s">
+        <v>143</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60" t="s">
+        <v>143</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="14">
+        <v>41948</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>52</v>
+      </c>
+      <c r="B62" t="s">
+        <v>143</v>
+      </c>
+      <c r="C62" s="14">
+        <v>41912</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1"/>
-    <hyperlink ref="C19" r:id="rId2"/>
-    <hyperlink ref="C20" r:id="rId3"/>
-    <hyperlink ref="C21" r:id="rId4"/>
+    <hyperlink ref="E8" r:id="rId1"/>
+    <hyperlink ref="C17" r:id="rId2"/>
+    <hyperlink ref="C16" r:id="rId3"/>
+    <hyperlink ref="C15" r:id="rId4"/>
+    <hyperlink ref="E22" r:id="rId5"/>
+    <hyperlink ref="E23" r:id="rId6"/>
+    <hyperlink ref="E24" r:id="rId7"/>
+    <hyperlink ref="E25" r:id="rId8"/>
+    <hyperlink ref="E26" r:id="rId9"/>
+    <hyperlink ref="E27" r:id="rId10"/>
+    <hyperlink ref="E28" r:id="rId11"/>
+    <hyperlink ref="E29" r:id="rId12"/>
+    <hyperlink ref="E30" r:id="rId13"/>
+    <hyperlink ref="E31" r:id="rId14"/>
+    <hyperlink ref="E32" r:id="rId15"/>
+    <hyperlink ref="C35" display="https://www.tadawul.com.sa/wps/portal/tadawul/market-participants/issuers/issuers-directory/company-details/!ut/p/z1/pdFLb4JAFAXg3-KC9RyGZ90hICBIQhWlszGDTRDDK4ba-O87Wjckldb07m7yncW5lzCSEdbwc1nwvmwbXon9jem72I9sHyYNPXetwNKdpf0aBxQA2d4ApbYpv6iIEBmyAB6CZKkqSB"/>
+    <hyperlink ref="C36" r:id="rId16"/>
+    <hyperlink ref="C37" r:id="rId17"/>
+    <hyperlink ref="C38" r:id="rId18"/>
+    <hyperlink ref="C39" r:id="rId19"/>
+    <hyperlink ref="E47" r:id="rId20" display="https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/hZFLU4NAEIR_DecdNrBBb8vKGxYNj8BeUhu1IhavA8aKv94N8aIWydym6uue7hokUIVEL4_NQU7N0MtW7bUgO-7HzAcLR5BzF-hTmTI7caIiImg7AxgzS78zIPYCvlYA9Uu3zFfgrZD4rXcAaJKG7sYMdSuGG3ow_ur_3xczEjx6hh4oxMqJDbRgMX_gmQ4m-QGuRbwKnDPMACwMhVsOJqpVzfViD4xRdvagnKcFZ07i8HzHi8R2Nqg2CCEWCpE4tMP-8pK3aRrvNdBgki_y86PVVALZ90xOqNKXgOehG2V_yk7dflAuGAOgsSsqaIJ3czx-xa9b-g3cxkle/dz/d5/L0lDUmlTUSEhL3dHa0FKRnNBLzROV3FpQSEhL2Vu/"/>
+    <hyperlink ref="E49" r:id="rId21" display="https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/hZBRT4MwFIV_yx543b0rbEPfOsJENzp1wKAvS1FkJKMQ7CT46y2YmJiIa596-52Tew5wiIFL8VHkQhWVFGf9TvjiyLyt46FNNhiwNdKnaOesfHcTbhZwGABCHHt2Y-H27p4tNUC9aB0FJqIF_JqeD8h_DgOAI4fiNYc5PADPz1X6nYfK1LRz4E32ljVZM700enxSqr410MC2bacE-zuVmTLwL8WpelcQ_yZ77sdEiVfRXs5azYWUjtC_szHgpSprIbt9V6aVXoQQREh0qcvR1giBfZ-ZMrYLmeP6LguOLPRX7jMklqVLgLqMsXgsD7aap535GVA6mXwBPc2OSw!!/dz/d5/L0lDUmlTUSEhL3dHa0FKRnNBLzROV3FpQSEhL2Vu/"/>
+    <hyperlink ref="E51" r:id="rId22"/>
+    <hyperlink ref="E52" r:id="rId23"/>
+    <hyperlink ref="E53" r:id="rId24" display="https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pVFNb4IwGP4tO3hc-rZUxN0qQ0GgbgIqXExxRFmgEEUN-_WraLJkifOw3vrk-WxRglYokeKUb0WTV1IU6h4n-prbnmmDQVwI-RjY-2JmjnzLjVwdLTsCIaaBhxS8icMHisDsxXgRagAUJf_RT7TfeguA-bPpeN6fYsMDpU86yl8NOgLcOQweOfRvBOdtQrGjWhihPgIWmR5_5QGGvv7AQa0IxB7Faurg7lsQgoKLD-N8FnHT8i0ernnkj6w5iikeEoqmKNkWVXr9ll3T1C896EEjPsT5WPTUDiGlKRq0wvcIm6qshWyDtkwr5UIIwK3WzzjuasAs7AK1fQyUokhW-1KFLk95dr6WPGRiv9mFbZ2hGF8AlVwdN2Ummxu4fu7wwzUp7pLqMlpB7nxSkRqtVpxKM_3KYvb0Df21EUM!/dz/d5/L0lHSkovd0RNQUZrQUVnQSEhLzROVkUvZW4!/"/>
+    <hyperlink ref="E54" r:id="rId25" display="https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pVFNb4IwGP4tO3hc-rZUZLtVhoJA3QRUuJjiiLJAIYoa_PWraLJkifOw3vrk-WxRgpYokeKYb0STV1IU6h4n-orbnmmDQVwI-QjYx3xqDn3LjVwdLToCIaaBXyh4Y4cPFIHZ89E81AAoSv6jH2u_9RYA86eT0aw_wYYHSp90lL8adAS4cxg8cujfCM77mGJHtTBCfQgsMj3-xgMMff2Bg1oRiB2K1dTB3bcgBAUXH8b5NOKm5Vs8XPHIH1ozFFNsUA1NULIpqvT6LdumqV970INGfIrToeipHUJKUzRoie8R1lVZC9kGbZlWyoUQgFutn3Hc1YBZ2AVq-xgoRZGsdqUKXRzz7HQtuc_Ebr0N2zpDMb4AKrk6rMtMNjdw9dzh-2tS3CXVZbSE3PmiIjVarTiWZnrOYvb0DZ3SUsU!/dz/d5/L0lHSkovd0RNQUZrQUVnQSEhLzROVkUvZW4!/"/>
+    <hyperlink ref="E55" r:id="rId26" display="https://www.tadawul.com.sa/wps/portal/tadawul/home/announcement-details/!ut/p/z1/pVFNb4IwGP4tO3hc-rZUZLtVhoJA3QRUuJjiiLJAIYoa_PWraLJkifOw3vrk-WxRgpYokeKYb0STV1IU6h4n-orbnmmDQVwI-QjYx3xqDn3LjVwdLToCIaaBXyh4Y4cPFIHZ89E81AAoSv6jH2u_9RYA86eT0aw_wYYHSp90lL8adAS4cxg8cujfCM77mGJHtTBCfQgsMj3-xgMMff2Bg1oRiB2K1dTB3bcgBAUXH8b5NOKm5Vs8XPHIH1ozFFNsgIYmKNkUVXr9lm3T1K896EEjPsXpUPTUDiGlKRq0xPcI66qshWyDtkwr5UIIwK3WzzjuasAs7AK1fQyUokhWu1KFLo55drqW3Gdit96GbZ2hGF8AlVwd1mUmmxu4eu7w_TUp7pLqMlpC7nxRkRqtVhxLMz1nMXv6Bp_kZcA!/dz/d5/L0lHSkovd0RNQUZrQUVnQSEhLzROVkUvZW4!/"/>
+    <hyperlink ref="E60" r:id="rId27"/>
+    <hyperlink ref="E61" r:id="rId28"/>
+    <hyperlink ref="E62" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add some classes with different logic
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/test_example.xlsx
+++ b/src/main/resources/templates/excel/test_example.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="195">
   <si>
     <t>BASIC INFO</t>
   </si>
@@ -395,9 +395,6 @@
   </si>
   <si>
     <t>1Arab National Bank</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
   <si>
     <t>Arabia Insurance Cooperative Co</t>
@@ -948,6 +945,24 @@
   </si>
   <si>
     <t>https://english.mubasher.info/news/2603212/Arabian-Pipes-wins-SAR-58-mln-contract-from-Aramco</t>
+  </si>
+  <si>
+    <t>Shareholding  test 2</t>
+  </si>
+  <si>
+    <t>SAR test 3</t>
+  </si>
+  <si>
+    <t>test  company address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test 2  company address  </t>
+  </si>
+  <si>
+    <t>www.anb2.com.sa</t>
+  </si>
+  <si>
+    <t>www.anb1.com.sa</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1107,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1132,6 +1147,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1437,7 +1453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -1677,10 +1693,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1937,10 +1953,10 @@
         <v>64</v>
       </c>
       <c r="U3" t="s">
-        <v>65</v>
+        <v>194</v>
       </c>
       <c r="V3" t="s">
-        <v>66</v>
+        <v>191</v>
       </c>
       <c r="X3" t="s">
         <v>67</v>
@@ -1952,6 +1968,83 @@
         <v>69</v>
       </c>
       <c r="AA3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="15">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4" s="15">
+        <v>1214</v>
+      </c>
+      <c r="H4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I4" t="s">
+        <v>190</v>
+      </c>
+      <c r="J4" s="16">
+        <v>31974</v>
+      </c>
+      <c r="K4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" t="s">
+        <v>97</v>
+      </c>
+      <c r="M4" t="s">
+        <v>102</v>
+      </c>
+      <c r="N4" t="s">
+        <v>101</v>
+      </c>
+      <c r="O4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" s="10">
+        <v>100</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>29190</v>
+      </c>
+      <c r="R4" t="s">
+        <v>103</v>
+      </c>
+      <c r="S4" t="s">
+        <v>63</v>
+      </c>
+      <c r="T4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U4" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="V4" t="s">
+        <v>192</v>
+      </c>
+      <c r="X4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA4" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1959,11 +2052,13 @@
   <hyperlinks>
     <hyperlink ref="T2" r:id="rId1" tooltip="info@anb.com.sa" display="mailto:info@anb.com.sa"/>
     <hyperlink ref="U2" r:id="rId2" display="http://www.anb.com.sa/"/>
-    <hyperlink ref="U3" r:id="rId3" display="http://www.anb.com.sa/"/>
-    <hyperlink ref="T3" r:id="rId4" tooltip="info@anb.com.sa" display="mailto:info@anb.com.sa"/>
+    <hyperlink ref="T3" r:id="rId3" tooltip="info@anb.com.sa" display="mailto:info@anb.com.sa"/>
+    <hyperlink ref="T4" r:id="rId4" tooltip="info@anb.com.sa" display="mailto:info@anb.com.sa"/>
+    <hyperlink ref="U4" r:id="rId5"/>
+    <hyperlink ref="U3" r:id="rId6" display="http://www.anb.com.sa/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1971,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2274,7 +2369,7 @@
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>42</v>
@@ -2294,16 +2389,16 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>108</v>
       </c>
       <c r="D19" s="17">
         <v>3.85E-2</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>94</v>
@@ -2314,7 +2409,7 @@
         <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2322,7 +2417,7 @@
         <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>43</v>
@@ -2339,16 +2434,16 @@
         <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C22" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -2356,16 +2451,16 @@
         <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2373,16 +2468,16 @@
         <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2390,16 +2485,16 @@
         <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25" s="14">
         <v>41251</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -2407,16 +2502,16 @@
         <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C26" s="14">
         <v>41182</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -2424,16 +2519,16 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C27" s="14">
         <v>41123</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2441,16 +2536,16 @@
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C28" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2458,16 +2553,16 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2475,16 +2570,16 @@
         <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C30" s="14">
         <v>40660</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -2492,16 +2587,16 @@
         <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C31" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -2509,16 +2604,16 @@
         <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C32" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -2526,7 +2621,7 @@
         <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -2534,7 +2629,7 @@
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>47</v>
@@ -2545,10 +2640,10 @@
         <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -2556,10 +2651,10 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -2567,10 +2662,10 @@
         <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -2578,10 +2673,10 @@
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -2589,10 +2684,10 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2600,7 +2695,7 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>42</v>
@@ -2620,19 +2715,19 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>144</v>
-      </c>
       <c r="D41" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2640,7 +2735,7 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2648,7 +2743,7 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>43</v>
@@ -2665,16 +2760,16 @@
         <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C44" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="E44" s="20" t="s">
         <v>146</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -2682,16 +2777,16 @@
         <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C45" s="14">
         <v>43219</v>
       </c>
       <c r="D45" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E45" s="20" t="s">
         <v>148</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -2699,16 +2794,16 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C46" s="14">
         <v>43069</v>
       </c>
       <c r="D46" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -2716,16 +2811,16 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C47" s="14">
         <v>42852</v>
       </c>
       <c r="D47" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E47" s="22" t="s">
         <v>152</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -2733,16 +2828,16 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C48" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="D48" s="21" t="s">
+      <c r="E48" s="20" t="s">
         <v>155</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2750,16 +2845,16 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C49" s="14">
         <v>42724</v>
       </c>
       <c r="D49" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E49" s="22" t="s">
         <v>157</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2767,16 +2862,16 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C50" s="14">
         <v>42683</v>
       </c>
       <c r="D50" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="E50" s="20" t="s">
         <v>159</v>
-      </c>
-      <c r="E50" s="20" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2784,16 +2879,16 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C51" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D51" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="D51" s="21" t="s">
+      <c r="E51" s="22" t="s">
         <v>162</v>
-      </c>
-      <c r="E51" s="22" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2801,16 +2896,16 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C52" s="14">
         <v>42473</v>
       </c>
       <c r="D52" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="E52" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="E52" s="22" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2818,16 +2913,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C53" s="14">
         <v>42466</v>
       </c>
       <c r="D53" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E53" s="22" t="s">
         <v>166</v>
-      </c>
-      <c r="E53" s="22" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2835,16 +2930,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C54" s="14">
         <v>42463</v>
       </c>
       <c r="D54" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="E54" s="22" t="s">
         <v>168</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2852,16 +2947,16 @@
         <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C55" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="D55" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="D55" s="21" t="s">
+      <c r="E55" s="22" t="s">
         <v>171</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2869,16 +2964,16 @@
         <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C56" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D56" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="D56" s="21" t="s">
+      <c r="E56" s="20" t="s">
         <v>174</v>
-      </c>
-      <c r="E56" s="20" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2886,16 +2981,16 @@
         <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C57" s="14">
         <v>42319</v>
       </c>
       <c r="D57" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="E57" s="20" t="s">
         <v>176</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2903,16 +2998,16 @@
         <v>52</v>
       </c>
       <c r="B58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C58" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D58" s="21" t="s">
+      <c r="E58" s="20" t="s">
         <v>179</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2920,16 +3015,16 @@
         <v>52</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C59" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="E59" s="20" t="s">
         <v>181</v>
-      </c>
-      <c r="D59" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2937,16 +3032,16 @@
         <v>52</v>
       </c>
       <c r="B60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C60" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D60" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="D60" s="21" t="s">
+      <c r="E60" s="22" t="s">
         <v>184</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2954,16 +3049,16 @@
         <v>52</v>
       </c>
       <c r="B61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C61" s="14">
         <v>41948</v>
       </c>
       <c r="D61" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E61" s="22" t="s">
         <v>186</v>
-      </c>
-      <c r="E61" s="22" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2971,16 +3066,16 @@
         <v>52</v>
       </c>
       <c r="B62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C62" s="14">
         <v>41912</v>
       </c>
       <c r="D62" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="E62" s="22" t="s">
         <v>188</v>
-      </c>
-      <c r="E62" s="22" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add few changes to templates
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/test_example.xlsx
+++ b/src/main/resources/templates/excel/test_example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="27700" windowHeight="17560" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="27700" windowHeight="17560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DESCRIPTION" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="103">
   <si>
     <t>BASIC INFO</t>
   </si>
@@ -374,6 +374,18 @@
   </si>
   <si>
     <t>provides commercial, Islamic, and investment banking services to individuals and corporate clients in Saudi Arabia</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>Riyadh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK TO PROFILE AT STOCK EXCHANGE </t>
+  </si>
+  <si>
+    <t>https://www.tadawul.com.sa/wps/portal/tadawul/market-participants/issuers/issuers-directory/company-details/!ut/p/z1/04_Sj9CPykssy0xPLMnMz0vMAfIjo8zi_Tx8nD0MLIy83V1DjA0czVx8nYP8PI0MDAz0I4EKzBEKDEJDLYEKjJ0DA11MjQzcTfW99KPSc_KTIGZllJQUWKkaqBqUJKYklpfmqBroRyXn5xYk5lUGV-Ym5QMVGRpYGOiHEzK1IDsop6zSUREALE4oLw!!/</t>
   </si>
 </sst>
 </file>
@@ -1054,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1075,26 +1087,28 @@
     <col min="11" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="31.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="106.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="80.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="71.1640625" customWidth="1"/>
-    <col min="28" max="28" width="50" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.5" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="32.1640625" customWidth="1"/>
+    <col min="21" max="21" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="109.5" customWidth="1"/>
+    <col min="25" max="25" width="14.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="71.1640625" customWidth="1"/>
+    <col min="30" max="30" width="50" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>50</v>
       </c>
@@ -1135,50 +1149,56 @@
         <v>95</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" s="4"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AD1" s="4"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1216,49 +1236,55 @@
         <v>98</v>
       </c>
       <c r="N2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O2" t="s">
         <v>94</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="10">
+      <c r="Q2" s="10">
         <v>4170</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="R2" s="11">
         <v>29190</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>62</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>102</v>
+      </c>
+      <c r="U2" t="s">
         <v>63</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>64</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>65</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>66</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>67</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>68</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>69</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" tooltip="info@anb.com.sa" display="mailto:info@anb.com.sa"/>
-    <hyperlink ref="U2" r:id="rId2" display="http://www.anb.com.sa/"/>
+    <hyperlink ref="V2" r:id="rId1" tooltip="info@anb.com.sa" display="mailto:info@anb.com.sa"/>
+    <hyperlink ref="W2" r:id="rId2" display="http://www.anb.com.sa/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1269,7 +1295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>